<commit_message>
added run.bat file and allure report
</commit_message>
<xml_diff>
--- a/Test_Data/Credkart_Test_Data.xlsx
+++ b/Test_Data/Credkart_Test_Data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="login_data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="login_data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>

</xml_diff>